<commit_message>
Punched a few items out
</commit_message>
<xml_diff>
--- a/punchlist.xlsx
+++ b/punchlist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="84" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,14 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Rpath punchlist</t>
   </si>
   <si>
-    <t>Updated 12/17/14</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -53,18 +50,27 @@
     <t>Sean</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t>S3 object</t>
   </si>
   <si>
     <t>Develop class definitions for ecopath object outputed from ecopath()</t>
   </si>
   <si>
+    <t>Done – created Rpath object in ecopath()</t>
+  </si>
+  <si>
     <t>summary(ecopath.obj)</t>
   </si>
   <si>
     <t>Develop output for summary function using ecopath object</t>
   </si>
   <si>
+    <t>First pass done</t>
+  </si>
+  <si>
     <t>plot(ecopath.obj)</t>
   </si>
   <si>
@@ -74,7 +80,7 @@
     <t>Convert to RCPP</t>
   </si>
   <si>
-    <t>The R package RCPP integrates R and C++ directly, may gain efficiency in ecosim() </t>
+    <t>The R package RCPP integrates R and C++ directly, may gain efficiency in ecosim()</t>
   </si>
   <si>
     <t>Rpath package</t>
@@ -143,7 +149,7 @@
     <t>?</t>
   </si>
   <si>
-    <t>C code already exists?</t>
+    <t>C code already exists? - Kerim may hire a programmer to do this next fall</t>
   </si>
 </sst>
 </file>
@@ -159,6 +165,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -180,6 +187,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -231,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,8 +280,12 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -304,7 +316,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -329,9 +341,6 @@
       <c r="F1" s="5"/>
     </row>
     <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
@@ -340,233 +349,249 @@
     </row>
     <row r="4" s="5" customFormat="true" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+    </row>
+    <row r="5" s="12" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" s="11" customFormat="true" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" s="11" customFormat="true" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="11" t="n">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="6" s="12" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" s="11" customFormat="true" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="7" s="12" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" s="11" customFormat="true" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="8" s="12" customFormat="true" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" s="11" customFormat="true" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="11" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="9" s="12" customFormat="true" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" s="11" customFormat="true" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" s="11" customFormat="true" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="11" t="n">
+        <v>42019</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="13" t="n">
+        <v>42013</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="12" t="n">
-        <v>42013</v>
-      </c>
-    </row>
-    <row r="12" s="11" customFormat="true" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="C12" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" s="11" customFormat="true" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="37.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="12" t="n">
+        <v>34</v>
+      </c>
+      <c r="F13" s="13" t="n">
         <v>42063</v>
       </c>
     </row>
-    <row r="14" s="11" customFormat="true" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="12" t="n">
+        <v>37</v>
+      </c>
+      <c r="F14" s="13" t="n">
         <v>42036</v>
       </c>
     </row>
-    <row r="15" s="11" customFormat="true" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="8"/>

</xml_diff>